<commit_message>
v1 completed. live prodcutıon production reports workcenter reports financial reports ( on progress )
</commit_message>
<xml_diff>
--- a/outputs(xlsx)/val2022.xlsx
+++ b/outputs(xlsx)/val2022.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -465,12 +465,12 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1439151.3135</v>
+        <v>1327657.3326</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -483,12 +483,12 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>681809.2533</v>
+        <v>936393.1359</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -501,12 +501,12 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>168542.10505</v>
+        <v>205409.71429</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -524,7 +524,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -542,7 +542,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -555,12 +555,12 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>13686.0877</v>
+        <v>12365.1962</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -573,12 +573,12 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>147844.3766</v>
+        <v>166632.3944</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -591,12 +591,12 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>290082.7237867053</v>
+        <v>267992.58430475</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -609,12 +609,12 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>473483.2750455245</v>
+        <v>288086.6466948192</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -627,12 +627,12 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>100614.62</v>
+        <v>94493.9105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -645,12 +645,12 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>294269.00624661</v>
+        <v>263078.2313484975</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -663,12 +663,12 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>163974.7207</v>
+        <v>155136.97005</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -681,12 +681,12 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>896886.7551</v>
+        <v>736319.0621</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -699,12 +699,12 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>29654.7032</v>
+        <v>34007.115</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -717,12 +717,12 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>90422.97500000001</v>
+        <v>110156.6828</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -735,12 +735,12 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>91225.2047</v>
+        <v>78389.03425</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -753,12 +753,12 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1188929.15932</v>
+        <v>1426041.0185</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -771,12 +771,12 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>100309.02434</v>
+        <v>51703.36268999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -789,12 +789,12 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>760473.7808773312</v>
+        <v>733340.2426935581</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -807,12 +807,12 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>71310.00771999999</v>
+        <v>72955.31894</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -830,7 +830,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -843,12 +843,12 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5914.933919999999</v>
+        <v>778.1121599999999</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -861,12 +861,12 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>23607.96144</v>
+        <v>24778.50914</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -879,12 +879,12 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>20342.2961</v>
+        <v>9519.626200000001</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -897,12 +897,12 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>26312.2412</v>
+        <v>14755.41242</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -915,12 +915,12 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>140557.0985</v>
+        <v>38243.71782</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -929,16 +929,16 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>KOMPPRC</t>
+          <t>SLDNGREED</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>14581.952</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -947,16 +947,16 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>PKOMPARC</t>
+          <t>VALFPLK</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>145938.23818</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SLDNGREED</t>
+          <t>WABCO-D</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>16084.852</v>
+        <v>853.9299999999999</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -983,29 +983,29 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>VALFPLK</t>
+          <t>WABCO-TR</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>140078.93165</v>
+        <v>14921.4646</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>MAMÜL</t>
+          <t>YARDIMCI MALZEME</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>VALFYPR</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>212.04</v>
       </c>
     </row>
     <row r="33">
@@ -1014,16 +1014,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MAMÜL</t>
+          <t>YARDIMCI MALZEME</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>WABCO-D</t>
+          <t>AMBALAJML</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>16180.43</v>
+        <v>251887.2495687281</v>
       </c>
     </row>
     <row r="34">
@@ -1032,21 +1032,21 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MAMÜL</t>
+          <t>YARDIMCI MALZEME</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>WABCO-TR</t>
+          <t>BAGCIVATA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>20400.77144</v>
+        <v>262836.2702344</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1055,16 +1055,16 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>BAGLANPIM</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>155743.3054937313</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1073,16 +1073,16 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ALS42-000</t>
+          <t>BAGLANTEL</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1691.0432</v>
+        <v>175.1560945</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1091,16 +1091,16 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>AMBALAJML</t>
+          <t>BAGLSOMUN</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>215139.3635471306</v>
+        <v>26986.4621684</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1109,16 +1109,16 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BAGCIVATA</t>
+          <t>BAGPERCIN</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>277366.6406096</v>
+        <v>173395.959</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1127,16 +1127,16 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BAGLANPIM</t>
+          <t>BAKIRPAST</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>159990.944814758</v>
+        <v>5917.950294984396</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1145,16 +1145,16 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>BAGLANTEL</t>
+          <t>CAPAKFIRC</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>177.2455881</v>
+        <v>7408.6306</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1163,16 +1163,16 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>BAGLSOMUN</t>
+          <t>CEKVALFPR</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>31160.1057504</v>
+        <v>193577.1112</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1181,16 +1181,16 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>BAGPERCIN</t>
+          <t>CIVATASBT</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>172899.809</v>
+        <v>1321.74</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1199,16 +1199,16 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BAKIRPAST</t>
+          <t>DDISKTASI</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1555.307481666996</v>
+        <v>619846.7193</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1217,16 +1217,16 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CAPAKFIRC</t>
+          <t>DIGER</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>13350.5224</v>
+        <v>378.04</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1235,16 +1235,16 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CEKVALFPR</t>
+          <t>ELEKTRONK</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>212903.5412</v>
+        <v>36722.37</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1253,16 +1253,16 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CIVATASBT</t>
+          <t>ENDUSTYAG</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1321.74</v>
+        <v>444761.56482</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1271,16 +1271,16 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>DDISKTASI</t>
+          <t>FILTKAGIT</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>622719.0724000001</v>
+        <v>2399.529</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1289,16 +1289,16 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ELEKTRONK</t>
+          <t>ISILISTUZ</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>36722.37</v>
+        <v>17200</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1307,16 +1307,16 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ENDUSTYAG</t>
+          <t>KESICIUCL</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>232050.31962</v>
+        <v>534857.424</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1325,16 +1325,16 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>FILTKAGIT</t>
+          <t>KIMYASIVI</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>414</v>
+        <v>3789.6638</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -1343,16 +1343,16 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>HFX12-000</t>
+          <t>KIRTASIYE</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>12833.3928</v>
+        <v>658.5474999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1361,16 +1361,16 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ISILISTUZ</t>
+          <t>KRDONANIM</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>6450</v>
+        <v>25191.7976</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1379,16 +1379,16 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>KESICIUCL</t>
+          <t>LASTIKPRC</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>468077.3436</v>
+        <v>26295.64026666961</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1397,16 +1397,16 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>KIMYASIVI</t>
+          <t>LAZERKESM</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2721.1788</v>
+        <v>795.1708000000001</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -1415,16 +1415,16 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>KIRTASIYE</t>
+          <t>PASONLJEL</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>328.0025</v>
+        <v>35666.667</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -1433,16 +1433,16 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>KRDONANIM</t>
+          <t>PASSPREYI</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>6424.8072</v>
+        <v>185.3712</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -1451,16 +1451,16 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>LASTIKPRC</t>
+          <t>PATLATMAT</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>29360.73</v>
+        <v>632.52</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1469,16 +1469,16 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MARKERKLM</t>
+          <t>PLAKACONT</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>43.332</v>
+        <v>68171.545</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -1487,16 +1487,16 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>OTKSGKCBK</t>
+          <t>PULBENZER</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>28113.6492</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -1505,16 +1505,16 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>PASONLJEL</t>
+          <t>SINAIGAZT</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>21813.30975</v>
+        <v>839.2952</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1523,16 +1523,16 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>PASSPREYI</t>
+          <t>SINTERCLK</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>185.3712</v>
+        <v>111337.8569</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -1541,16 +1541,16 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>PATLATMAT</t>
+          <t>TELKALIPM</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>903.5999999999999</v>
+        <v>1659.8181</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -1559,16 +1559,16 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>PLAKACONT</t>
+          <t>TEMIZMALZ</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>68172.095</v>
+        <v>53.94</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -1577,16 +1577,16 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>PULBENZER</t>
+          <t>VALVEPLAT</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>29838.26</v>
+        <v>12225.201</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -1595,16 +1595,16 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SINAIGAZT</t>
+          <t>VCP11-000</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>419.6476</v>
+        <v>3138.23</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -1613,16 +1613,16 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SINTERCLK</t>
+          <t>YARDIMCI</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>131132.6652</v>
+        <v>117.008</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -1631,16 +1631,16 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>TELKALIPM</t>
+          <t>YAYPARCAS</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>159.8181</v>
+        <v>167480.643</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -1649,16 +1649,16 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>TELRECINE</t>
+          <t>YUZEYTASI</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>636.14</v>
+        <v>62962.77</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -1667,16 +1667,16 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>TEMIZMALZ</t>
+          <t>ZIMPARAML</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>21.39</v>
+        <v>7900.5477</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -1685,160 +1685,160 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>VALVEPLAT</t>
+          <t>ZIMPATOZU</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>8729.448999999999</v>
+        <v>53588.416</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>YARDIMCI MALZEME</t>
+          <t>YARI MAMÜL</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>VCP11-000</t>
+          <t>AMORPRC</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>8268.76</v>
+        <v>791655.6014542505</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>YARDIMCI MALZEME</t>
+          <t>YARI MAMÜL</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>YAPISTIRI</t>
+          <t>CHKVLF</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>37.505</v>
+        <v>7098.96</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>YARDIMCI MALZEME</t>
+          <t>YARI MAMÜL</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>YAYPARCAS</t>
+          <t>DDMETAL</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>186753.5175</v>
+        <v>9401.8766</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>YARDIMCI MALZEME</t>
+          <t>YARI MAMÜL</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>YCK30-000</t>
+          <t>DIGER</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>763.9399999999998</v>
+        <v>79843.77976533616</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>YARDIMCI MALZEME</t>
+          <t>YARI MAMÜL</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>YCK30-500</t>
+          <t>KOMPPRC</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>3999.125</v>
+        <v>929217.8657</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>YARDIMCI MALZEME</t>
+          <t>YARI MAMÜL</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>YUZEYTASI</t>
+          <t>PKOMPARC</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>52942.33</v>
+        <v>26415.176</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>YARDIMCI MALZEME</t>
+          <t>YARI MAMÜL</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>ZIMPARAML</t>
+          <t>VALFPLK</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>7944.225</v>
+        <v>916863.9790624588</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>YARDIMCI MALZEME</t>
+          <t>YARI MAMÜL</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>ZIMPATOZU</t>
+          <t>VALFYPR</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>9416.944</v>
+        <v>93105.7249</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -1847,155 +1847,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>AMORPRC</t>
+          <t>YAY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>258552.3507727487</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>YARI MAMÜL</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>CHKVLF</t>
-        </is>
-      </c>
-      <c r="D80" t="n">
-        <v>13342.32</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>YARI MAMÜL</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>DDMETAL</t>
-        </is>
-      </c>
-      <c r="D81" t="n">
-        <v>9750.167000000001</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>YARI MAMÜL</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>DIGER</t>
-        </is>
-      </c>
-      <c r="D82" t="n">
-        <v>4099.884</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>YARI MAMÜL</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>KOMPPRC</t>
-        </is>
-      </c>
-      <c r="D83" t="n">
-        <v>942867.5679</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>YARI MAMÜL</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>PKOMPARC</t>
-        </is>
-      </c>
-      <c r="D84" t="n">
-        <v>23816.8287</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>YARI MAMÜL</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>VALFPLK</t>
-        </is>
-      </c>
-      <c r="D85" t="n">
-        <v>850902.5535528268</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>YARI MAMÜL</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>VALFYPR</t>
-        </is>
-      </c>
-      <c r="D86" t="n">
-        <v>96010.3704</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>YARI MAMÜL</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>YAY</t>
-        </is>
-      </c>
-      <c r="D87" t="n">
-        <v>61058.9062</v>
+        <v>76745.8177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>